<commit_message>
Added more screenshots and steps up to 30 to LabVIEW Install Documentation/Main Document/LabVIEW Install Documentation.docx
</commit_message>
<xml_diff>
--- a/LabVIEW Install Documentation/Supporting Documents/Configurations/Configuration Matrix.xlsx
+++ b/LabVIEW Install Documentation/Supporting Documents/Configurations/Configuration Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mysite.jci.com/personal/jbeachsc_jci_com/Documents/Documents/Projects/LabVIEW Install Documentation/Supporting Documents/Configurations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2780" documentId="8_{F0CA27F2-6703-47B6-838F-C7D756A64328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D84DE02-AC3E-4935-BE6D-6AA65B56EF46}"/>
+  <xr:revisionPtr revIDLastSave="2781" documentId="8_{F0CA27F2-6703-47B6-838F-C7D756A64328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FDBA6FA-0CFD-4F90-8184-8D2193F2F78C}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-345" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4AB76D6F-471E-4DF4-A309-9E739330102C}"/>
   </bookViews>
@@ -28904,7 +28904,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -28940,7 +28940,7 @@
       </c>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -28976,7 +28976,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>267</v>
       </c>
@@ -29012,7 +29012,7 @@
       </c>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>267</v>
       </c>
@@ -29048,7 +29048,7 @@
       </c>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>267</v>
       </c>
@@ -29084,7 +29084,7 @@
       </c>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>267</v>
       </c>
@@ -29156,7 +29156,7 @@
       </c>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
@@ -29192,7 +29192,7 @@
       </c>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
@@ -29228,7 +29228,7 @@
       </c>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>0</v>
       </c>
@@ -29264,7 +29264,7 @@
       </c>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -29300,7 +29300,7 @@
       </c>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>0</v>
       </c>
@@ -29336,7 +29336,7 @@
       </c>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>0</v>
       </c>
@@ -29372,7 +29372,7 @@
       </c>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>0</v>
       </c>
@@ -29408,7 +29408,7 @@
       </c>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>0</v>
       </c>
@@ -29444,7 +29444,7 @@
       </c>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>0</v>
       </c>
@@ -29516,7 +29516,7 @@
       </c>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>0</v>
       </c>
@@ -29552,7 +29552,7 @@
       </c>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>0</v>
       </c>
@@ -29588,7 +29588,7 @@
       </c>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>0</v>
       </c>
@@ -29660,7 +29660,7 @@
       </c>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>0</v>
       </c>
@@ -29696,7 +29696,7 @@
       </c>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>0</v>
       </c>
@@ -29732,7 +29732,7 @@
       </c>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>0</v>
       </c>
@@ -29804,7 +29804,7 @@
       </c>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>0</v>
       </c>
@@ -29840,7 +29840,7 @@
       </c>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>0</v>
       </c>
@@ -29876,7 +29876,7 @@
       </c>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>0</v>
       </c>
@@ -29912,7 +29912,7 @@
       </c>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>0</v>
       </c>
@@ -29948,7 +29948,7 @@
       </c>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>0</v>
       </c>
@@ -29984,7 +29984,7 @@
       </c>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="34" t="s">
         <v>96</v>
       </c>
@@ -30020,7 +30020,7 @@
       </c>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
         <v>96</v>
       </c>
@@ -30056,7 +30056,7 @@
       </c>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
         <v>96</v>
       </c>
@@ -30128,7 +30128,7 @@
       </c>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>0</v>
       </c>
@@ -30164,7 +30164,7 @@
       </c>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>0</v>
       </c>
@@ -30200,7 +30200,7 @@
       </c>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>0</v>
       </c>
@@ -30560,7 +30560,7 @@
       </c>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>96</v>
       </c>
@@ -30596,7 +30596,7 @@
       </c>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>96</v>
       </c>
@@ -30632,7 +30632,7 @@
       </c>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="26" t="s">
         <v>0</v>
       </c>
@@ -30668,7 +30668,7 @@
       </c>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>0</v>
       </c>
@@ -30704,7 +30704,7 @@
       </c>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>0</v>
       </c>
@@ -30740,7 +30740,7 @@
       </c>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>0</v>
       </c>
@@ -30812,7 +30812,7 @@
       </c>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>0</v>
       </c>
@@ -30848,7 +30848,7 @@
       </c>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
         <v>0</v>
       </c>
@@ -30884,7 +30884,7 @@
       </c>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>0</v>
       </c>
@@ -30920,7 +30920,7 @@
       </c>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>0</v>
       </c>
@@ -30956,7 +30956,7 @@
       </c>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>0</v>
       </c>
@@ -30992,7 +30992,7 @@
       </c>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>0</v>
       </c>
@@ -31028,7 +31028,7 @@
       </c>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>0</v>
       </c>
@@ -31100,7 +31100,7 @@
       </c>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>0</v>
       </c>
@@ -31136,7 +31136,7 @@
       </c>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>0</v>
       </c>
@@ -31172,7 +31172,7 @@
       </c>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>0</v>
       </c>
@@ -31208,7 +31208,7 @@
       </c>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="28" t="s">
         <v>96</v>
       </c>
@@ -31316,7 +31316,7 @@
       </c>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>0</v>
       </c>
@@ -31388,7 +31388,7 @@
       </c>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>0</v>
       </c>
@@ -31424,7 +31424,7 @@
       </c>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>0</v>
       </c>
@@ -31460,7 +31460,7 @@
       </c>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>0</v>
       </c>
@@ -31496,7 +31496,7 @@
       </c>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="28" t="s">
         <v>96</v>
       </c>
@@ -31532,7 +31532,7 @@
       </c>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>0</v>
       </c>
@@ -31568,7 +31568,7 @@
       </c>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>0</v>
       </c>
@@ -31604,7 +31604,7 @@
       </c>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="26" t="s">
         <v>0</v>
       </c>
@@ -31748,7 +31748,7 @@
       </c>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>0</v>
       </c>
@@ -31784,7 +31784,7 @@
       </c>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>0</v>
       </c>
@@ -31820,7 +31820,7 @@
       </c>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="28" t="s">
         <v>96</v>
       </c>
@@ -31856,7 +31856,7 @@
       </c>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>0</v>
       </c>
@@ -31892,7 +31892,7 @@
       </c>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>0</v>
       </c>
@@ -31928,7 +31928,7 @@
       </c>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
         <v>96</v>
       </c>
@@ -31964,7 +31964,7 @@
       </c>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
         <v>96</v>
       </c>
@@ -32000,7 +32000,7 @@
       </c>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>0</v>
       </c>
@@ -32036,7 +32036,7 @@
       </c>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>0</v>
       </c>
@@ -32072,7 +32072,7 @@
       </c>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>0</v>
       </c>
@@ -32108,7 +32108,7 @@
       </c>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>0</v>
       </c>
@@ -32144,7 +32144,7 @@
       </c>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="26" t="s">
         <v>0</v>
       </c>
@@ -32180,7 +32180,7 @@
       </c>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="28" t="s">
         <v>96</v>
       </c>
@@ -34746,11 +34746,6 @@
         <filter val="Corey"/>
         <filter val="Garrett"/>
         <filter val="Spencer"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="LabVIEW"/>
       </filters>
     </filterColumn>
     <filterColumn colId="2">

</xml_diff>